<commit_message>
Missed a few things in MESAT conversions
</commit_message>
<xml_diff>
--- a/genSpacecraft/DownlinkSpecMESAT1.xlsx
+++ b/genSpacecraft/DownlinkSpecMESAT1.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1461" uniqueCount="549">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1462" uniqueCount="550">
   <si>
     <t xml:space="preserve">//</t>
   </si>
@@ -374,7 +374,7 @@
     <t xml:space="preserve">uint8_t</t>
   </si>
   <si>
-    <t xml:space="preserve">8_bit_temp|INVALID_BYTE</t>
+    <t xml:space="preserve">8_bit_temp|INVALID_TEMP</t>
   </si>
   <si>
     <t xml:space="preserve">Host Temp 1</t>
@@ -611,7 +611,7 @@
     <t xml:space="preserve">hostCANVolts0</t>
   </si>
   <si>
-    <t xml:space="preserve">ten_volt_8_bit</t>
+    <t xml:space="preserve">ten_volt_8_bit|INVALID_10_VOLTS</t>
   </si>
   <si>
     <t xml:space="preserve">Host Bat Volts 1</t>
@@ -642,6 +642,9 @@
   </si>
   <si>
     <t xml:space="preserve">hostCANVolts3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mesat_batt_current</t>
   </si>
   <si>
     <t xml:space="preserve">Host Bat Volts 4</t>
@@ -2045,8 +2048,8 @@
   </sheetPr>
   <dimension ref="A1:Q1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A51" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G56" activeCellId="0" sqref="G56:G59"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A56" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H69" activeCellId="0" sqref="H69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4375,7 +4378,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="37.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B56" s="31" t="s">
         <v>171</v>
       </c>
@@ -5062,11 +5065,13 @@
       </c>
       <c r="F69" s="23"/>
       <c r="G69" s="22" t="s">
-        <v>161</v>
-      </c>
-      <c r="H69" s="22"/>
+        <v>207</v>
+      </c>
+      <c r="H69" s="22" t="s">
+        <v>145</v>
+      </c>
       <c r="I69" s="32" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="J69" s="29" t="n">
         <f aca="false">J68+D68</f>
@@ -5099,10 +5104,10 @@
     </row>
     <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B70" s="31" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C70" s="32" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="D70" s="32" t="n">
         <v>8</v>
@@ -5116,7 +5121,7 @@
       </c>
       <c r="H70" s="22"/>
       <c r="I70" s="32" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="J70" s="29" t="n">
         <f aca="false">J69+D69</f>
@@ -5149,10 +5154,10 @@
     </row>
     <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B71" s="31" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C71" s="32" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="D71" s="32" t="n">
         <v>8</v>
@@ -5166,7 +5171,7 @@
       </c>
       <c r="H71" s="22"/>
       <c r="I71" s="32" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="J71" s="29" t="n">
         <f aca="false">J70+D70</f>
@@ -5202,10 +5207,10 @@
         <v>1</v>
       </c>
       <c r="B72" s="31" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="C72" s="32" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="D72" s="32" t="n">
         <v>8</v>
@@ -5219,7 +5224,7 @@
       </c>
       <c r="H72" s="22"/>
       <c r="I72" s="32" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="J72" s="29" t="n">
         <f aca="false">J71+D71</f>
@@ -5252,10 +5257,10 @@
     </row>
     <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B73" s="31" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="C73" s="32" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="D73" s="32" t="n">
         <v>8</v>
@@ -5271,7 +5276,7 @@
         <v>77</v>
       </c>
       <c r="I73" s="32" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="J73" s="29" t="n">
         <f aca="false">J72+D72</f>
@@ -5304,10 +5309,10 @@
     </row>
     <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B74" s="31" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="C74" s="32" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="D74" s="32" t="n">
         <v>8</v>
@@ -5323,7 +5328,7 @@
         <v>77</v>
       </c>
       <c r="I74" s="32" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="J74" s="29" t="n">
         <f aca="false">J73+D73</f>
@@ -5342,7 +5347,7 @@
         <v>11.5</v>
       </c>
       <c r="N74" s="1" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="O74" s="24" t="n">
         <v>9</v>
@@ -5356,10 +5361,10 @@
     </row>
     <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B75" s="31" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="C75" s="32" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="D75" s="32" t="n">
         <v>8</v>
@@ -5375,7 +5380,7 @@
         <v>77</v>
       </c>
       <c r="I75" s="32" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="J75" s="29" t="n">
         <f aca="false">J74+D74</f>
@@ -5394,7 +5399,7 @@
         <v>11.75</v>
       </c>
       <c r="N75" s="1" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="O75" s="24" t="n">
         <v>9</v>
@@ -5408,10 +5413,10 @@
     </row>
     <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B76" s="31" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="C76" s="32" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="D76" s="32" t="n">
         <v>8</v>
@@ -5427,7 +5432,7 @@
         <v>77</v>
       </c>
       <c r="I76" s="32" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="J76" s="29" t="n">
         <f aca="false">J75+D75</f>
@@ -5446,7 +5451,7 @@
         <v>12</v>
       </c>
       <c r="N76" s="1" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="O76" s="24" t="n">
         <v>9</v>
@@ -5460,10 +5465,10 @@
     </row>
     <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B77" s="31" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="C77" s="32" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="D77" s="32" t="n">
         <v>8</v>
@@ -5479,7 +5484,7 @@
         <v>77</v>
       </c>
       <c r="I77" s="32" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="J77" s="29" t="n">
         <f aca="false">J76+D76</f>
@@ -5498,7 +5503,7 @@
         <v>12.25</v>
       </c>
       <c r="N77" s="1" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="O77" s="24" t="n">
         <v>9</v>
@@ -5512,10 +5517,10 @@
     </row>
     <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B78" s="31" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="C78" s="32" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="D78" s="32" t="n">
         <v>8</v>
@@ -5531,7 +5536,7 @@
         <v>77</v>
       </c>
       <c r="I78" s="32" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="J78" s="29" t="n">
         <f aca="false">J77+D77</f>
@@ -5550,7 +5555,7 @@
         <v>12.5</v>
       </c>
       <c r="N78" s="1" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="O78" s="24" t="n">
         <v>9</v>
@@ -5564,10 +5569,10 @@
     </row>
     <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B79" s="31" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="C79" s="32" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="D79" s="32" t="n">
         <v>8</v>
@@ -5583,7 +5588,7 @@
         <v>77</v>
       </c>
       <c r="I79" s="32" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="J79" s="29" t="n">
         <f aca="false">J78+D78</f>
@@ -5616,10 +5621,10 @@
     </row>
     <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B80" s="31" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="C80" s="32" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="D80" s="32" t="n">
         <v>8</v>
@@ -5635,7 +5640,7 @@
         <v>77</v>
       </c>
       <c r="I80" s="32" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="J80" s="29" t="n">
         <f aca="false">J79+D79</f>
@@ -5654,7 +5659,7 @@
         <v>13</v>
       </c>
       <c r="N80" s="1" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="O80" s="24" t="n">
         <v>9</v>
@@ -5668,10 +5673,10 @@
     </row>
     <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B81" s="31" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="C81" s="31" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="D81" s="32" t="n">
         <v>8</v>
@@ -5685,7 +5690,7 @@
       </c>
       <c r="H81" s="22"/>
       <c r="I81" s="32" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="J81" s="29" t="n">
         <f aca="false">J80+D80</f>
@@ -5718,10 +5723,10 @@
     </row>
     <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B82" s="31" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="C82" s="31" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="D82" s="32" t="n">
         <v>16</v>
@@ -5735,7 +5740,7 @@
       </c>
       <c r="H82" s="22"/>
       <c r="I82" s="32" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="J82" s="29" t="n">
         <f aca="false">J81+D81</f>
@@ -5778,7 +5783,7 @@
       <c r="G83" s="23"/>
       <c r="H83" s="23"/>
       <c r="I83" s="23" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="J83" s="29" t="n">
         <f aca="false">J82+D82</f>
@@ -5816,7 +5821,7 @@
         <v>0</v>
       </c>
       <c r="B85" s="7" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="C85" s="7"/>
       <c r="D85" s="7"/>
@@ -5828,7 +5833,7 @@
     </row>
     <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="1" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="B86" s="31"/>
       <c r="C86" s="32"/>
@@ -5845,10 +5850,10 @@
     </row>
     <row r="87" customFormat="false" ht="25.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B87" s="31" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="C87" s="32" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="D87" s="32" t="n">
         <v>8</v>
@@ -5857,16 +5862,16 @@
         <v>26</v>
       </c>
       <c r="F87" s="23" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="G87" s="22" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="H87" s="22" t="s">
         <v>27</v>
       </c>
       <c r="I87" s="23" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="J87" s="29" t="n">
         <f aca="false">J83</f>
@@ -5899,10 +5904,10 @@
     </row>
     <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B88" s="31" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="C88" s="31" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="D88" s="32" t="n">
         <v>8</v>
@@ -5916,7 +5921,7 @@
       </c>
       <c r="H88" s="22"/>
       <c r="I88" s="32" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="J88" s="29" t="n">
         <f aca="false">J87+D87</f>
@@ -5955,7 +5960,7 @@
       <c r="C89" s="32"/>
       <c r="D89" s="32"/>
       <c r="E89" s="23" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="F89" s="23"/>
       <c r="G89" s="23"/>
@@ -5968,10 +5973,10 @@
     </row>
     <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B90" s="31" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="C90" s="31" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="D90" s="32" t="n">
         <v>1</v>
@@ -5985,7 +5990,7 @@
       </c>
       <c r="H90" s="22"/>
       <c r="I90" s="32" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="J90" s="29" t="n">
         <f aca="false">J88+D88</f>
@@ -6018,10 +6023,10 @@
     </row>
     <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B91" s="31" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="C91" s="32" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="D91" s="32" t="n">
         <v>1</v>
@@ -6037,7 +6042,7 @@
         <v>27</v>
       </c>
       <c r="I91" s="23" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="J91" s="29" t="n">
         <f aca="false">J90+D90</f>
@@ -6070,10 +6075,10 @@
     </row>
     <row r="92" customFormat="false" ht="25.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B92" s="31" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="C92" s="32" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="D92" s="32" t="n">
         <v>1</v>
@@ -6089,7 +6094,7 @@
         <v>27</v>
       </c>
       <c r="I92" s="23" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="J92" s="29" t="n">
         <f aca="false">J91+D91</f>
@@ -6122,10 +6127,10 @@
     </row>
     <row r="93" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B93" s="31" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="C93" s="32" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="D93" s="32" t="n">
         <v>1</v>
@@ -6141,7 +6146,7 @@
         <v>27</v>
       </c>
       <c r="I93" s="23" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="J93" s="29" t="n">
         <f aca="false">J92+D92</f>
@@ -6174,10 +6179,10 @@
     </row>
     <row r="94" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B94" s="31" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="C94" s="32" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="D94" s="32" t="n">
         <v>1</v>
@@ -6193,7 +6198,7 @@
         <v>27</v>
       </c>
       <c r="I94" s="23" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="J94" s="29" t="n">
         <f aca="false">J93+D93</f>
@@ -6226,10 +6231,10 @@
     </row>
     <row r="95" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B95" s="31" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="C95" s="32" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="D95" s="32" t="n">
         <v>1</v>
@@ -6276,10 +6281,10 @@
     </row>
     <row r="96" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B96" s="33" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="C96" s="32" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="D96" s="32" t="n">
         <v>1</v>
@@ -6295,7 +6300,7 @@
         <v>27</v>
       </c>
       <c r="I96" s="23" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="J96" s="29" t="n">
         <f aca="false">J95+D95</f>
@@ -6328,10 +6333,10 @@
     </row>
     <row r="97" customFormat="false" ht="25.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B97" s="33" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="C97" s="32" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="D97" s="32" t="n">
         <v>1</v>
@@ -6341,13 +6346,13 @@
       </c>
       <c r="F97" s="23"/>
       <c r="G97" s="22" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="H97" s="22" t="s">
         <v>27</v>
       </c>
       <c r="I97" s="23" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="J97" s="29" t="n">
         <f aca="false">J96+D96</f>
@@ -6400,10 +6405,10 @@
     </row>
     <row r="99" customFormat="false" ht="50.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B99" s="31" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="C99" s="32" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="D99" s="32" t="n">
         <v>8</v>
@@ -6419,7 +6424,7 @@
         <v>27</v>
       </c>
       <c r="I99" s="23" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="J99" s="29" t="n">
         <f aca="false">J97+D97</f>
@@ -6452,10 +6457,10 @@
     </row>
     <row r="100" customFormat="false" ht="75.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B100" s="31" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="C100" s="32" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="D100" s="32" t="n">
         <v>8</v>
@@ -6471,7 +6476,7 @@
         <v>27</v>
       </c>
       <c r="I100" s="23" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="J100" s="29" t="n">
         <f aca="false">J99+D99</f>
@@ -6504,10 +6509,10 @@
     </row>
     <row r="101" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B101" s="31" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="C101" s="32" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="D101" s="32" t="n">
         <v>32</v>
@@ -6525,7 +6530,7 @@
         <v>27</v>
       </c>
       <c r="I101" s="23" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="J101" s="29" t="n">
         <f aca="false">J100+D100</f>
@@ -6558,10 +6563,10 @@
     </row>
     <row r="102" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B102" s="31" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="C102" s="32" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="D102" s="32" t="n">
         <v>8</v>
@@ -6577,7 +6582,7 @@
         <v>27</v>
       </c>
       <c r="I102" s="23" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="J102" s="29" t="n">
         <f aca="false">J101+D101</f>
@@ -6610,10 +6615,10 @@
     </row>
     <row r="103" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B103" s="31" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="C103" s="32" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="D103" s="32" t="n">
         <v>8</v>
@@ -6629,7 +6634,7 @@
         <v>27</v>
       </c>
       <c r="I103" s="23" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="J103" s="29" t="n">
         <f aca="false">J102+D102</f>
@@ -6662,10 +6667,10 @@
     </row>
     <row r="104" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B104" s="31" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="C104" s="32" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="D104" s="32" t="n">
         <v>8</v>
@@ -6675,13 +6680,13 @@
       </c>
       <c r="F104" s="23"/>
       <c r="G104" s="23" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="H104" s="22" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="I104" s="23" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="J104" s="29" t="n">
         <f aca="false">J103+D103</f>
@@ -6700,7 +6705,7 @@
         <v>16.75</v>
       </c>
       <c r="N104" s="1" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="O104" s="3" t="n">
         <v>9</v>
@@ -6714,10 +6719,10 @@
     </row>
     <row r="105" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B105" s="31" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="C105" s="32" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="D105" s="32" t="n">
         <v>1</v>
@@ -6727,13 +6732,13 @@
       </c>
       <c r="F105" s="23"/>
       <c r="G105" s="22" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="H105" s="22" t="s">
         <v>27</v>
       </c>
       <c r="I105" s="32" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="J105" s="29" t="n">
         <f aca="false">J104+D104</f>
@@ -6752,7 +6757,7 @@
         <v>17</v>
       </c>
       <c r="N105" s="1" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="O105" s="3" t="n">
         <v>8</v>
@@ -6766,10 +6771,10 @@
     </row>
     <row r="106" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B106" s="31" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="C106" s="32" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="D106" s="32" t="n">
         <v>1</v>
@@ -6779,7 +6784,7 @@
       </c>
       <c r="F106" s="23"/>
       <c r="G106" s="22" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="H106" s="22" t="s">
         <v>27</v>
@@ -6802,7 +6807,7 @@
         <v>17.03125</v>
       </c>
       <c r="N106" s="1" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="O106" s="3" t="n">
         <v>8</v>
@@ -6816,10 +6821,10 @@
     </row>
     <row r="107" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B107" s="31" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="C107" s="32" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="D107" s="32" t="n">
         <v>1</v>
@@ -6829,7 +6834,7 @@
       </c>
       <c r="F107" s="23"/>
       <c r="G107" s="22" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="H107" s="22" t="s">
         <v>27</v>
@@ -6852,7 +6857,7 @@
         <v>17.0625</v>
       </c>
       <c r="N107" s="1" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="O107" s="3" t="n">
         <v>8</v>
@@ -6866,10 +6871,10 @@
     </row>
     <row r="108" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B108" s="31" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="C108" s="32" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="D108" s="32" t="n">
         <v>1</v>
@@ -6879,7 +6884,7 @@
       </c>
       <c r="F108" s="23"/>
       <c r="G108" s="22" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="H108" s="22" t="s">
         <v>27</v>
@@ -6902,7 +6907,7 @@
         <v>17.09375</v>
       </c>
       <c r="N108" s="1" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="O108" s="3" t="n">
         <v>8</v>
@@ -6916,10 +6921,10 @@
     </row>
     <row r="109" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B109" s="31" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="C109" s="32" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="D109" s="32" t="n">
         <v>1</v>
@@ -6929,7 +6934,7 @@
       </c>
       <c r="F109" s="23"/>
       <c r="G109" s="22" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="H109" s="22" t="s">
         <v>27</v>
@@ -6952,7 +6957,7 @@
         <v>17.125</v>
       </c>
       <c r="N109" s="1" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="O109" s="24" t="n">
         <v>8</v>
@@ -6966,10 +6971,10 @@
     </row>
     <row r="110" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B110" s="31" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="C110" s="32" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="D110" s="32" t="n">
         <v>1</v>
@@ -6979,7 +6984,7 @@
       </c>
       <c r="F110" s="23"/>
       <c r="G110" s="22" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="H110" s="22" t="s">
         <v>27</v>
@@ -7002,7 +7007,7 @@
         <v>17.15625</v>
       </c>
       <c r="N110" s="1" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="O110" s="24" t="n">
         <v>8</v>
@@ -7016,10 +7021,10 @@
     </row>
     <row r="111" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B111" s="31" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="C111" s="32" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="D111" s="32" t="n">
         <v>1</v>
@@ -7029,7 +7034,7 @@
       </c>
       <c r="F111" s="23"/>
       <c r="G111" s="22" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="H111" s="22" t="s">
         <v>27</v>
@@ -7052,7 +7057,7 @@
         <v>17.1875</v>
       </c>
       <c r="N111" s="1" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="O111" s="24" t="n">
         <v>8</v>
@@ -7066,10 +7071,10 @@
     </row>
     <row r="112" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B112" s="31" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="C112" s="32" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="D112" s="32" t="n">
         <v>1</v>
@@ -7079,7 +7084,7 @@
       </c>
       <c r="F112" s="23"/>
       <c r="G112" s="22" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="H112" s="22" t="s">
         <v>27</v>
@@ -7102,7 +7107,7 @@
         <v>17.21875</v>
       </c>
       <c r="N112" s="1" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="O112" s="24" t="n">
         <v>8</v>
@@ -7116,10 +7121,10 @@
     </row>
     <row r="113" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B113" s="31" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="C113" s="32" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="D113" s="32" t="n">
         <v>1</v>
@@ -7129,13 +7134,13 @@
       </c>
       <c r="F113" s="23"/>
       <c r="G113" s="22" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="H113" s="22" t="s">
         <v>27</v>
       </c>
       <c r="I113" s="32" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="J113" s="29" t="n">
         <f aca="false">J112+D112</f>
@@ -7154,7 +7159,7 @@
         <v>17.25</v>
       </c>
       <c r="N113" s="1" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="O113" s="24" t="n">
         <v>8</v>
@@ -7168,10 +7173,10 @@
     </row>
     <row r="114" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B114" s="31" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="C114" s="32" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="D114" s="32" t="n">
         <v>1</v>
@@ -7181,7 +7186,7 @@
       </c>
       <c r="F114" s="23"/>
       <c r="G114" s="22" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="H114" s="22" t="s">
         <v>27</v>
@@ -7204,7 +7209,7 @@
         <v>17.28125</v>
       </c>
       <c r="N114" s="1" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="O114" s="24" t="n">
         <v>8</v>
@@ -7218,10 +7223,10 @@
     </row>
     <row r="115" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B115" s="31" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="C115" s="32" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="D115" s="32" t="n">
         <v>1</v>
@@ -7231,7 +7236,7 @@
       </c>
       <c r="F115" s="23"/>
       <c r="G115" s="22" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="H115" s="22" t="s">
         <v>27</v>
@@ -7254,7 +7259,7 @@
         <v>17.3125</v>
       </c>
       <c r="N115" s="1" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="O115" s="24" t="n">
         <v>8</v>
@@ -7268,10 +7273,10 @@
     </row>
     <row r="116" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B116" s="31" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="C116" s="32" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="D116" s="32" t="n">
         <v>1</v>
@@ -7281,7 +7286,7 @@
       </c>
       <c r="F116" s="23"/>
       <c r="G116" s="22" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="H116" s="22" t="s">
         <v>27</v>
@@ -7304,7 +7309,7 @@
         <v>17.34375</v>
       </c>
       <c r="N116" s="1" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="O116" s="24" t="n">
         <v>8</v>
@@ -7318,10 +7323,10 @@
     </row>
     <row r="117" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B117" s="31" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="C117" s="32" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="D117" s="32" t="n">
         <v>1</v>
@@ -7331,7 +7336,7 @@
       </c>
       <c r="F117" s="23"/>
       <c r="G117" s="22" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="H117" s="22" t="s">
         <v>27</v>
@@ -7354,7 +7359,7 @@
         <v>17.375</v>
       </c>
       <c r="N117" s="1" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="O117" s="24" t="n">
         <v>8</v>
@@ -7368,10 +7373,10 @@
     </row>
     <row r="118" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B118" s="31" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="C118" s="32" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="D118" s="32" t="n">
         <v>1</v>
@@ -7381,7 +7386,7 @@
       </c>
       <c r="F118" s="23"/>
       <c r="G118" s="22" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="H118" s="22" t="s">
         <v>27</v>
@@ -7404,7 +7409,7 @@
         <v>17.40625</v>
       </c>
       <c r="N118" s="1" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="O118" s="24" t="n">
         <v>8</v>
@@ -7418,10 +7423,10 @@
     </row>
     <row r="119" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B119" s="31" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="C119" s="32" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="D119" s="32" t="n">
         <v>1</v>
@@ -7431,7 +7436,7 @@
       </c>
       <c r="F119" s="23"/>
       <c r="G119" s="22" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="H119" s="22" t="s">
         <v>27</v>
@@ -7454,7 +7459,7 @@
         <v>17.4375</v>
       </c>
       <c r="N119" s="1" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="O119" s="24" t="n">
         <v>8</v>
@@ -7468,10 +7473,10 @@
     </row>
     <row r="120" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B120" s="31" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="C120" s="32" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="D120" s="32" t="n">
         <v>1</v>
@@ -7481,7 +7486,7 @@
       </c>
       <c r="F120" s="23"/>
       <c r="G120" s="22" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="H120" s="22" t="s">
         <v>27</v>
@@ -7504,7 +7509,7 @@
         <v>17.46875</v>
       </c>
       <c r="N120" s="1" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="O120" s="24" t="n">
         <v>8</v>
@@ -7518,10 +7523,10 @@
     </row>
     <row r="121" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B121" s="31" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="C121" s="32" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="D121" s="32" t="n">
         <v>1</v>
@@ -7531,13 +7536,13 @@
       </c>
       <c r="F121" s="23"/>
       <c r="G121" s="22" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="H121" s="22" t="s">
         <v>27</v>
       </c>
       <c r="I121" s="32" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="J121" s="29" t="n">
         <f aca="false">J120+D120</f>
@@ -7556,7 +7561,7 @@
         <v>17.5</v>
       </c>
       <c r="N121" s="1" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="O121" s="24" t="n">
         <v>8</v>
@@ -7570,10 +7575,10 @@
     </row>
     <row r="122" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B122" s="31" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="C122" s="32" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="D122" s="32" t="n">
         <v>1</v>
@@ -7583,7 +7588,7 @@
       </c>
       <c r="F122" s="23"/>
       <c r="G122" s="22" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="H122" s="22" t="s">
         <v>27</v>
@@ -7606,7 +7611,7 @@
         <v>17.53125</v>
       </c>
       <c r="N122" s="1" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="O122" s="24" t="n">
         <v>8</v>
@@ -7620,10 +7625,10 @@
     </row>
     <row r="123" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B123" s="31" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="C123" s="32" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="D123" s="32" t="n">
         <v>1</v>
@@ -7633,7 +7638,7 @@
       </c>
       <c r="F123" s="23"/>
       <c r="G123" s="22" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="H123" s="22" t="s">
         <v>27</v>
@@ -7656,7 +7661,7 @@
         <v>17.5625</v>
       </c>
       <c r="N123" s="1" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="O123" s="24" t="n">
         <v>8</v>
@@ -7670,10 +7675,10 @@
     </row>
     <row r="124" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B124" s="31" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="C124" s="32" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="D124" s="32" t="n">
         <v>1</v>
@@ -7683,7 +7688,7 @@
       </c>
       <c r="F124" s="23"/>
       <c r="G124" s="22" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="H124" s="22" t="s">
         <v>27</v>
@@ -7706,7 +7711,7 @@
         <v>17.59375</v>
       </c>
       <c r="N124" s="1" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="O124" s="24" t="n">
         <v>8</v>
@@ -7720,10 +7725,10 @@
     </row>
     <row r="125" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B125" s="31" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="C125" s="32" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="D125" s="32" t="n">
         <v>1</v>
@@ -7733,7 +7738,7 @@
       </c>
       <c r="F125" s="23"/>
       <c r="G125" s="22" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="H125" s="22" t="s">
         <v>27</v>
@@ -7756,7 +7761,7 @@
         <v>17.625</v>
       </c>
       <c r="N125" s="1" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="O125" s="24" t="n">
         <v>8</v>
@@ -7770,10 +7775,10 @@
     </row>
     <row r="126" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B126" s="31" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="C126" s="32" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="D126" s="32" t="n">
         <v>1</v>
@@ -7783,7 +7788,7 @@
       </c>
       <c r="F126" s="23"/>
       <c r="G126" s="22" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="H126" s="22" t="s">
         <v>27</v>
@@ -7820,10 +7825,10 @@
     </row>
     <row r="127" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B127" s="31" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="C127" s="32" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="D127" s="32" t="n">
         <v>1</v>
@@ -7833,11 +7838,11 @@
       </c>
       <c r="F127" s="23"/>
       <c r="G127" s="22" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="H127" s="22"/>
       <c r="I127" s="32" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="J127" s="29" t="n">
         <f aca="false">J126+D126</f>
@@ -7856,7 +7861,7 @@
         <v>17.6875</v>
       </c>
       <c r="N127" s="1" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="O127" s="24" t="n">
         <v>9</v>
@@ -7870,10 +7875,10 @@
     </row>
     <row r="128" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B128" s="31" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="C128" s="32" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="D128" s="32" t="n">
         <v>1</v>
@@ -7883,7 +7888,7 @@
       </c>
       <c r="F128" s="23"/>
       <c r="G128" s="22" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="H128" s="22" t="s">
         <v>27</v>
@@ -7906,7 +7911,7 @@
         <v>17.71875</v>
       </c>
       <c r="N128" s="1" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="O128" s="24" t="n">
         <v>9</v>
@@ -7920,10 +7925,10 @@
     </row>
     <row r="129" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B129" s="31" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="C129" s="32" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="D129" s="32" t="n">
         <v>1</v>
@@ -7933,7 +7938,7 @@
       </c>
       <c r="F129" s="23"/>
       <c r="G129" s="22" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="H129" s="22" t="s">
         <v>27</v>
@@ -7970,10 +7975,10 @@
     </row>
     <row r="130" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B130" s="31" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="C130" s="32" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="D130" s="32" t="n">
         <v>1</v>
@@ -7983,7 +7988,7 @@
       </c>
       <c r="F130" s="23"/>
       <c r="G130" s="22" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="H130" s="22" t="s">
         <v>27</v>
@@ -8020,10 +8025,10 @@
     </row>
     <row r="131" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B131" s="31" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="C131" s="32" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="D131" s="32" t="n">
         <v>1</v>
@@ -8033,7 +8038,7 @@
       </c>
       <c r="F131" s="23"/>
       <c r="G131" s="22" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="H131" s="22" t="s">
         <v>27</v>
@@ -8070,10 +8075,10 @@
     </row>
     <row r="132" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B132" s="31" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="C132" s="32" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="D132" s="32" t="n">
         <v>1</v>
@@ -8083,7 +8088,7 @@
       </c>
       <c r="F132" s="23"/>
       <c r="G132" s="22" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="H132" s="22" t="s">
         <v>27</v>
@@ -8120,10 +8125,10 @@
     </row>
     <row r="133" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B133" s="31" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="C133" s="32" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="D133" s="32" t="n">
         <v>1</v>
@@ -8133,7 +8138,7 @@
       </c>
       <c r="F133" s="23"/>
       <c r="G133" s="22" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="H133" s="22" t="s">
         <v>27</v>
@@ -8170,10 +8175,10 @@
     </row>
     <row r="134" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B134" s="31" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="C134" s="32" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="D134" s="32" t="n">
         <v>1</v>
@@ -8183,7 +8188,7 @@
       </c>
       <c r="F134" s="23"/>
       <c r="G134" s="22" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="H134" s="22" t="s">
         <v>27</v>
@@ -8220,10 +8225,10 @@
     </row>
     <row r="135" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B135" s="31" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="C135" s="32" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="D135" s="32" t="n">
         <v>1</v>
@@ -8233,7 +8238,7 @@
       </c>
       <c r="F135" s="23"/>
       <c r="G135" s="22" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="H135" s="22" t="s">
         <v>27</v>
@@ -8270,10 +8275,10 @@
     </row>
     <row r="136" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B136" s="31" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="C136" s="32" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="D136" s="32" t="n">
         <v>1</v>
@@ -8283,7 +8288,7 @@
       </c>
       <c r="F136" s="23"/>
       <c r="G136" s="22" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="H136" s="22" t="s">
         <v>27</v>
@@ -8306,7 +8311,7 @@
         <v>17.96875</v>
       </c>
       <c r="N136" s="1" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="O136" s="24" t="n">
         <v>8</v>
@@ -8320,10 +8325,10 @@
     </row>
     <row r="137" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B137" s="31" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="C137" s="32" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="D137" s="32" t="n">
         <v>8</v>
@@ -8339,7 +8344,7 @@
         <v>27</v>
       </c>
       <c r="I137" s="23" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="J137" s="29" t="n">
         <f aca="false">J136+D136</f>
@@ -8372,10 +8377,10 @@
     </row>
     <row r="138" customFormat="false" ht="37.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B138" s="31" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="C138" s="32" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="D138" s="32" t="n">
         <v>8</v>
@@ -8391,7 +8396,7 @@
         <v>27</v>
       </c>
       <c r="I138" s="23" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="J138" s="29" t="n">
         <f aca="false">J137+D137</f>
@@ -8424,10 +8429,10 @@
     </row>
     <row r="139" customFormat="false" ht="25.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B139" s="31" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="C139" s="32" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="D139" s="32" t="n">
         <v>8</v>
@@ -8443,7 +8448,7 @@
         <v>27</v>
       </c>
       <c r="I139" s="23" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="J139" s="29" t="n">
         <f aca="false">J138+D138</f>
@@ -8476,10 +8481,10 @@
     </row>
     <row r="140" customFormat="false" ht="37.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B140" s="31" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="C140" s="32" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="D140" s="32" t="n">
         <v>8</v>
@@ -8495,7 +8500,7 @@
         <v>27</v>
       </c>
       <c r="I140" s="23" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="J140" s="29" t="n">
         <f aca="false">J139+D139</f>
@@ -8528,10 +8533,10 @@
     </row>
     <row r="141" customFormat="false" ht="25.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B141" s="31" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="C141" s="32" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="D141" s="32" t="n">
         <v>8</v>
@@ -8547,7 +8552,7 @@
         <v>27</v>
       </c>
       <c r="I141" s="23" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="J141" s="29" t="n">
         <f aca="false">J140+D140</f>
@@ -8580,10 +8585,10 @@
     </row>
     <row r="142" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B142" s="31" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="C142" s="32" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="D142" s="32" t="n">
         <v>8</v>
@@ -8597,7 +8602,7 @@
       </c>
       <c r="H142" s="22"/>
       <c r="I142" s="32" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="J142" s="29" t="n">
         <f aca="false">J141+D141</f>
@@ -8630,10 +8635,10 @@
     </row>
     <row r="143" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B143" s="31" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="C143" s="32" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="D143" s="32" t="n">
         <v>8</v>
@@ -8647,7 +8652,7 @@
       </c>
       <c r="H143" s="22"/>
       <c r="I143" s="32" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="J143" s="29" t="n">
         <f aca="false">J142+D142</f>
@@ -8680,10 +8685,10 @@
     </row>
     <row r="144" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B144" s="31" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="C144" s="32" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="D144" s="32" t="n">
         <v>8</v>
@@ -8697,7 +8702,7 @@
       </c>
       <c r="H144" s="22"/>
       <c r="I144" s="32" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="J144" s="29" t="n">
         <f aca="false">J143+D143</f>
@@ -8730,10 +8735,10 @@
     </row>
     <row r="145" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B145" s="31" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="C145" s="32" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="D145" s="32" t="n">
         <v>8</v>
@@ -8747,7 +8752,7 @@
       </c>
       <c r="H145" s="22"/>
       <c r="I145" s="32" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="J145" s="29" t="n">
         <f aca="false">J144+D144</f>
@@ -8780,10 +8785,10 @@
     </row>
     <row r="146" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B146" s="31" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="C146" s="32" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="D146" s="32" t="n">
         <v>8</v>
@@ -8797,7 +8802,7 @@
       </c>
       <c r="H146" s="22"/>
       <c r="I146" s="32" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="J146" s="29" t="n">
         <f aca="false">J145+D145</f>
@@ -8830,10 +8835,10 @@
     </row>
     <row r="147" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B147" s="31" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="C147" s="32" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="D147" s="32" t="n">
         <v>8</v>
@@ -8847,7 +8852,7 @@
       </c>
       <c r="H147" s="22"/>
       <c r="I147" s="32" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="J147" s="29" t="n">
         <f aca="false">J146+D146</f>
@@ -8902,10 +8907,10 @@
     </row>
     <row r="149" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B149" s="31" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="C149" s="31" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="D149" s="32" t="n">
         <v>1</v>
@@ -8921,7 +8926,7 @@
         <v>27</v>
       </c>
       <c r="I149" s="23" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="J149" s="29" t="n">
         <f aca="false">J148+D148</f>
@@ -8951,10 +8956,10 @@
     </row>
     <row r="150" customFormat="false" ht="50.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B150" s="31" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="C150" s="32" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="D150" s="32" t="n">
         <v>1</v>
@@ -8970,7 +8975,7 @@
         <v>27</v>
       </c>
       <c r="I150" s="23" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="J150" s="29" t="n">
         <f aca="false">J149+D149</f>
@@ -9003,10 +9008,10 @@
     </row>
     <row r="151" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B151" s="31" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="C151" s="32" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="D151" s="32" t="n">
         <v>3</v>
@@ -9016,7 +9021,7 @@
       </c>
       <c r="F151" s="23"/>
       <c r="G151" s="23" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="H151" s="22" t="s">
         <v>27</v>
@@ -9053,10 +9058,10 @@
     </row>
     <row r="152" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B152" s="31" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="C152" s="32" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="D152" s="32" t="n">
         <v>1</v>
@@ -9103,10 +9108,10 @@
     </row>
     <row r="153" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B153" s="31" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="C153" s="32" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="D153" s="32" t="n">
         <v>1</v>
@@ -9122,7 +9127,7 @@
         <v>27</v>
       </c>
       <c r="I153" s="23" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="J153" s="29" t="n">
         <f aca="false">J152+D152</f>
@@ -9155,10 +9160,10 @@
     </row>
     <row r="154" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B154" s="31" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="C154" s="32" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="D154" s="32" t="n">
         <v>1</v>
@@ -9174,7 +9179,7 @@
         <v>27</v>
       </c>
       <c r="I154" s="23" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="J154" s="29" t="n">
         <f aca="false">J153+D153</f>
@@ -9227,10 +9232,10 @@
     </row>
     <row r="156" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B156" s="31" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="C156" s="31" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="D156" s="32" t="n">
         <v>8</v>
@@ -9244,7 +9249,7 @@
       </c>
       <c r="H156" s="22"/>
       <c r="I156" s="32" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="J156" s="29" t="n">
         <f aca="false">J155+D155</f>
@@ -9277,10 +9282,10 @@
     </row>
     <row r="157" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B157" s="31" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="C157" s="31" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="D157" s="32" t="n">
         <v>8</v>
@@ -9294,7 +9299,7 @@
       </c>
       <c r="H157" s="22"/>
       <c r="I157" s="32" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="J157" s="29" t="n">
         <f aca="false">J156+D156</f>
@@ -9327,10 +9332,10 @@
     </row>
     <row r="158" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B158" s="31" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="C158" s="31" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D158" s="32" t="n">
         <v>8</v>
@@ -9344,7 +9349,7 @@
       </c>
       <c r="H158" s="22"/>
       <c r="I158" s="32" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="J158" s="29" t="n">
         <f aca="false">J157+D157</f>
@@ -9377,10 +9382,10 @@
     </row>
     <row r="159" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B159" s="31" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="C159" s="31" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="D159" s="32" t="n">
         <v>8</v>
@@ -9394,7 +9399,7 @@
       </c>
       <c r="H159" s="22"/>
       <c r="I159" s="32" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="J159" s="29" t="n">
         <f aca="false">J158+D158</f>
@@ -9437,7 +9442,7 @@
       <c r="G160" s="36"/>
       <c r="H160" s="35"/>
       <c r="I160" s="36" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="J160" s="29" t="n">
         <f aca="false">J159+D159</f>
@@ -9464,7 +9469,7 @@
     </row>
     <row r="163" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A163" s="1" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="B163" s="31"/>
       <c r="C163" s="32"/>
@@ -9484,7 +9489,7 @@
         <v>57</v>
       </c>
       <c r="C164" s="32" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D164" s="32" t="n">
         <v>32</v>
@@ -9542,7 +9547,7 @@
       <c r="G165" s="36"/>
       <c r="H165" s="35"/>
       <c r="I165" s="36" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="J165" s="29" t="n">
         <f aca="false">J164+D164</f>
@@ -9579,31 +9584,31 @@
     </row>
     <row r="167" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A167" s="1" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
     </row>
     <row r="168" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B168" s="31" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="C168" s="32" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="D168" s="27" t="n">
         <v>32</v>
       </c>
       <c r="E168" s="38" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="F168" s="23"/>
       <c r="G168" s="0" t="n">
         <v>0</v>
       </c>
       <c r="H168" s="3" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="I168" s="28" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="J168" s="29" t="n">
         <f aca="false">J83</f>
@@ -9636,10 +9641,10 @@
     </row>
     <row r="169" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B169" s="31" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="C169" s="32" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="D169" s="27" t="n">
         <v>16</v>
@@ -9649,11 +9654,11 @@
       </c>
       <c r="F169" s="23"/>
       <c r="G169" s="23" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="H169" s="0"/>
       <c r="I169" s="28" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="J169" s="29" t="n">
         <f aca="false">J168+D168</f>
@@ -9672,7 +9677,7 @@
         <v>15</v>
       </c>
       <c r="N169" s="1" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="O169" s="3" t="n">
         <v>5</v>
@@ -9686,16 +9691,16 @@
     </row>
     <row r="170" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B170" s="31" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="C170" s="32" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="D170" s="27" t="n">
         <v>8</v>
       </c>
       <c r="E170" s="38" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="F170" s="23"/>
       <c r="G170" s="23" t="n">
@@ -9705,7 +9710,7 @@
         <v>27</v>
       </c>
       <c r="I170" s="28" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="J170" s="29" t="n">
         <f aca="false">J169+D169</f>
@@ -9724,7 +9729,7 @@
         <v>15.5</v>
       </c>
       <c r="N170" s="1" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="O170" s="3" t="n">
         <v>5</v>
@@ -9738,10 +9743,10 @@
     </row>
     <row r="171" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B171" s="31" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="C171" s="32" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="D171" s="27" t="n">
         <v>8</v>
@@ -9755,7 +9760,7 @@
         <v>27</v>
       </c>
       <c r="I171" s="28" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="J171" s="29" t="n">
         <f aca="false">J170+D170</f>
@@ -9797,7 +9802,7 @@
       <c r="G172" s="36"/>
       <c r="H172" s="35"/>
       <c r="I172" s="36" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="J172" s="29" t="n">
         <f aca="false">J171+D171</f>
@@ -9818,15 +9823,15 @@
     </row>
     <row r="175" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A175" s="1" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
     </row>
     <row r="176" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B176" s="31" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="C176" s="32" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="D176" s="27" t="n">
         <v>32</v>
@@ -9838,7 +9843,7 @@
       </c>
       <c r="H176" s="0"/>
       <c r="I176" s="28" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="J176" s="29" t="n">
         <f aca="false">J83</f>
@@ -9871,10 +9876,10 @@
     </row>
     <row r="177" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B177" s="31" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="C177" s="32" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="D177" s="27" t="n">
         <v>16</v>
@@ -9884,10 +9889,10 @@
       </c>
       <c r="F177" s="23"/>
       <c r="G177" s="23" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="I177" s="28" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="J177" s="29" t="n">
         <f aca="false">J176+D176</f>
@@ -9906,7 +9911,7 @@
         <v>15</v>
       </c>
       <c r="N177" s="1" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="O177" s="3" t="n">
         <v>5</v>
@@ -9920,10 +9925,10 @@
     </row>
     <row r="178" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B178" s="31" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="C178" s="32" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="D178" s="27" t="n">
         <v>16</v>
@@ -9931,10 +9936,10 @@
       <c r="E178" s="38"/>
       <c r="F178" s="23"/>
       <c r="G178" s="23" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="I178" s="28" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="J178" s="29" t="n">
         <f aca="false">J177+D177</f>
@@ -9953,7 +9958,7 @@
         <v>15.5</v>
       </c>
       <c r="N178" s="1" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="O178" s="3" t="n">
         <v>5</v>
@@ -9967,10 +9972,10 @@
     </row>
     <row r="179" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B179" s="0" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="C179" s="32" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="D179" s="27" t="n">
         <v>32</v>
@@ -9981,7 +9986,7 @@
         <v>36</v>
       </c>
       <c r="I179" s="28" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="J179" s="29" t="n">
         <f aca="false">J178+D178</f>
@@ -10014,16 +10019,16 @@
     </row>
     <row r="180" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B180" s="31" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="C180" s="32" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="D180" s="27" t="n">
         <v>8</v>
       </c>
       <c r="E180" s="38" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="F180" s="23"/>
       <c r="G180" s="23" t="n">
@@ -10033,7 +10038,7 @@
         <v>27</v>
       </c>
       <c r="I180" s="28" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="J180" s="29" t="n">
         <f aca="false">J179+D179</f>
@@ -10052,7 +10057,7 @@
         <v>17</v>
       </c>
       <c r="N180" s="1" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="O180" s="3" t="n">
         <v>5</v>
@@ -10066,10 +10071,10 @@
     </row>
     <row r="181" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B181" s="31" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="C181" s="32" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="D181" s="27" t="n">
         <v>24</v>
@@ -10126,7 +10131,7 @@
       <c r="G182" s="36"/>
       <c r="H182" s="35"/>
       <c r="I182" s="36" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="J182" s="29" t="n">
         <f aca="false">J181+D181</f>
@@ -10152,15 +10157,15 @@
     </row>
     <row r="186" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A186" s="1" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
     </row>
     <row r="187" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B187" s="31" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="C187" s="32" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="D187" s="27" t="n">
         <v>32</v>
@@ -10173,10 +10178,10 @@
         <v>1</v>
       </c>
       <c r="H187" s="40" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="I187" s="28" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="J187" s="29" t="n">
         <f aca="false">J160</f>
@@ -10209,10 +10214,10 @@
     </row>
     <row r="188" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B188" s="31" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="C188" s="32" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="D188" s="27" t="n">
         <v>16</v>
@@ -10222,13 +10227,13 @@
       </c>
       <c r="F188" s="23"/>
       <c r="G188" s="23" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="H188" s="40" t="s">
         <v>27</v>
       </c>
       <c r="I188" s="28" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="J188" s="29" t="n">
         <f aca="false">J187+D187</f>
@@ -10247,7 +10252,7 @@
         <v>23</v>
       </c>
       <c r="N188" s="1" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="O188" s="3" t="n">
         <v>5</v>
@@ -10261,10 +10266,10 @@
     </row>
     <row r="189" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B189" s="31" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="C189" s="32" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="D189" s="27" t="n">
         <v>8</v>
@@ -10274,13 +10279,13 @@
       </c>
       <c r="F189" s="23"/>
       <c r="G189" s="40" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="H189" s="22" t="s">
         <v>27</v>
       </c>
       <c r="I189" s="28" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="J189" s="29" t="n">
         <f aca="false">J188+D188</f>
@@ -10299,7 +10304,7 @@
         <v>23.5</v>
       </c>
       <c r="N189" s="5" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="O189" s="24" t="n">
         <v>5</v>
@@ -10489,7 +10494,7 @@
         <v>55</v>
       </c>
       <c r="C194" s="22" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="D194" s="22" t="n">
         <v>5</v>
@@ -10557,7 +10562,7 @@
       </c>
       <c r="B196" s="31"/>
       <c r="I196" s="1" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="J196" s="29" t="n">
         <f aca="false">J194+D194</f>
@@ -10578,7 +10583,7 @@
     </row>
     <row r="197" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A197" s="41" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="B197" s="11"/>
       <c r="C197" s="42"/>
@@ -10644,10 +10649,10 @@
     </row>
     <row r="199" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B199" s="31" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="C199" s="22" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="D199" s="22" t="n">
         <v>5248</v>
@@ -10665,7 +10670,7 @@
         <v>27</v>
       </c>
       <c r="I199" s="23" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="J199" s="4" t="n">
         <v>0</v>
@@ -10697,10 +10702,10 @@
     </row>
     <row r="200" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B200" s="31" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="C200" s="22" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="D200" s="22" t="n">
         <v>7</v>
@@ -10749,10 +10754,10 @@
     </row>
     <row r="201" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B201" s="31" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="C201" s="22" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="D201" s="22" t="n">
         <v>1</v>
@@ -10766,7 +10771,7 @@
       </c>
       <c r="H201" s="22"/>
       <c r="I201" s="23" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="J201" s="4" t="n">
         <f aca="false">J200+D200</f>
@@ -10785,7 +10790,7 @@
         <v>164.21875</v>
       </c>
       <c r="N201" s="1" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="O201" s="3" t="n">
         <v>1</v>
@@ -10802,7 +10807,7 @@
         <v>59</v>
       </c>
       <c r="I202" s="1" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="J202" s="4" t="n">
         <f aca="false">J201+D201</f>
@@ -10830,7 +10835,7 @@
     </row>
     <row r="204" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A204" s="43" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="B204" s="11"/>
       <c r="C204" s="42"/>
@@ -10896,10 +10901,10 @@
     </row>
     <row r="206" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B206" s="31" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="C206" s="22" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="D206" s="22" t="n">
         <v>664</v>
@@ -10917,7 +10922,7 @@
         <v>27</v>
       </c>
       <c r="I206" s="23" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="J206" s="4" t="n">
         <v>0</v>
@@ -10949,10 +10954,10 @@
     </row>
     <row r="207" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B207" s="31" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="C207" s="22" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
       <c r="D207" s="22" t="n">
         <v>7</v>
@@ -11001,10 +11006,10 @@
     </row>
     <row r="208" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B208" s="31" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="C208" s="22" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="D208" s="22" t="n">
         <v>1</v>
@@ -11018,7 +11023,7 @@
       </c>
       <c r="H208" s="22"/>
       <c r="I208" s="23" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="J208" s="4" t="n">
         <f aca="false">J207+D207</f>
@@ -11037,7 +11042,7 @@
         <v>20.96875</v>
       </c>
       <c r="N208" s="1" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="O208" s="3" t="n">
         <v>1</v>
@@ -11054,7 +11059,7 @@
         <v>59</v>
       </c>
       <c r="I209" s="1" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="J209" s="4" t="n">
         <f aca="false">J208+D208</f>
@@ -11075,7 +11080,7 @@
     </row>
     <row r="213" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A213" s="43" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
       <c r="B213" s="11"/>
       <c r="C213" s="42"/>
@@ -11141,10 +11146,10 @@
     </row>
     <row r="215" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B215" s="31" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="C215" s="32" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="D215" s="27" t="n">
         <v>32</v>
@@ -11157,10 +11162,10 @@
         <v>1</v>
       </c>
       <c r="H215" s="40" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="I215" s="28" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="J215" s="4" t="n">
         <f aca="false">J209</f>
@@ -11193,10 +11198,10 @@
     </row>
     <row r="216" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B216" s="31" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="C216" s="32" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="D216" s="27" t="n">
         <v>16</v>
@@ -11205,16 +11210,16 @@
         <v>26</v>
       </c>
       <c r="F216" s="23" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="G216" s="23" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="H216" s="40" t="s">
         <v>27</v>
       </c>
       <c r="I216" s="28" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="J216" s="4" t="n">
         <f aca="false">J215+D215</f>
@@ -11233,7 +11238,7 @@
         <v>22</v>
       </c>
       <c r="N216" s="1" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="O216" s="3" t="n">
         <v>2</v>
@@ -11247,10 +11252,10 @@
     </row>
     <row r="217" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B217" s="31" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="C217" s="32" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="D217" s="27" t="n">
         <v>8</v>
@@ -11258,13 +11263,13 @@
       <c r="E217" s="38"/>
       <c r="F217" s="23"/>
       <c r="G217" s="40" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="H217" s="40" t="s">
         <v>27</v>
       </c>
       <c r="I217" s="28" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="J217" s="4" t="n">
         <f aca="false">J216+D216</f>
@@ -11283,7 +11288,7 @@
         <v>22.5</v>
       </c>
       <c r="N217" s="5" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="O217" s="24" t="n">
         <v>2</v>
@@ -11300,7 +11305,7 @@
         <v>28</v>
       </c>
       <c r="C218" s="32" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="D218" s="27" t="n">
         <v>8</v>
@@ -11314,7 +11319,7 @@
         <v>27</v>
       </c>
       <c r="I218" s="28" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="J218" s="4" t="n">
         <f aca="false">J217+D217</f>
@@ -11350,7 +11355,7 @@
         <v>59</v>
       </c>
       <c r="I219" s="1" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="J219" s="4" t="n">
         <f aca="false">J218+D218</f>
@@ -11383,7 +11388,7 @@
     </row>
     <row r="221" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A221" s="43" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
     </row>
     <row r="222" s="14" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11441,10 +11446,10 @@
     </row>
     <row r="223" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B223" s="44" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="C223" s="38" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="D223" s="38" t="n">
         <v>32</v>
@@ -11457,10 +11462,10 @@
         <v>161</v>
       </c>
       <c r="H223" s="38" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="I223" s="38" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="J223" s="45" t="n">
         <v>0</v>
@@ -11478,7 +11483,7 @@
         <v>0</v>
       </c>
       <c r="N223" s="1" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="O223" s="3" t="n">
         <v>1</v>
@@ -11492,10 +11497,10 @@
     </row>
     <row r="224" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B224" s="44" t="s">
-        <v>470</v>
+        <v>471</v>
       </c>
       <c r="C224" s="38" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="D224" s="38" t="n">
         <v>32</v>
@@ -11508,10 +11513,10 @@
         <v>161</v>
       </c>
       <c r="H224" s="38" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="I224" s="38" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="J224" s="45" t="n">
         <f aca="false">J223+D223</f>
@@ -11530,7 +11535,7 @@
         <v>1</v>
       </c>
       <c r="N224" s="1" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="O224" s="3" t="n">
         <v>1</v>
@@ -11544,7 +11549,7 @@
     </row>
     <row r="225" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A225" s="1" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="B225" s="44"/>
       <c r="C225" s="38"/>
@@ -11561,10 +11566,10 @@
     </row>
     <row r="226" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B226" s="44" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="C226" s="38" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="D226" s="38" t="n">
         <v>1</v>
@@ -11574,13 +11579,13 @@
       </c>
       <c r="F226" s="38"/>
       <c r="G226" s="38" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="H226" s="38" t="s">
         <v>27</v>
       </c>
       <c r="I226" s="38" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="J226" s="45" t="n">
         <f aca="false">J224+D224</f>
@@ -11599,7 +11604,7 @@
         <v>2</v>
       </c>
       <c r="N226" s="1" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="O226" s="3" t="n">
         <v>1</v>
@@ -11613,10 +11618,10 @@
     </row>
     <row r="227" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B227" s="44" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="C227" s="38" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="D227" s="38" t="n">
         <v>5</v>
@@ -11630,7 +11635,7 @@
       </c>
       <c r="H227" s="38"/>
       <c r="I227" s="38" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="J227" s="45" t="n">
         <f aca="false">J226+D226</f>
@@ -11649,7 +11654,7 @@
         <v>2.03125</v>
       </c>
       <c r="N227" s="1" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="O227" s="3" t="n">
         <v>1</v>
@@ -11663,10 +11668,10 @@
     </row>
     <row r="228" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B228" s="44" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="C228" s="38" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="D228" s="38" t="n">
         <v>4</v>
@@ -11682,7 +11687,7 @@
         <v>27</v>
       </c>
       <c r="I228" s="38" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="J228" s="45" t="n">
         <f aca="false">J227+D227</f>
@@ -11701,7 +11706,7 @@
         <v>2.1875</v>
       </c>
       <c r="N228" s="1" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="O228" s="3" t="n">
         <v>1</v>
@@ -11715,10 +11720,10 @@
     </row>
     <row r="229" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B229" s="44" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
       <c r="C229" s="38" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
       <c r="D229" s="38" t="n">
         <v>5</v>
@@ -11734,7 +11739,7 @@
         <v>27</v>
       </c>
       <c r="I229" s="38" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="J229" s="45" t="n">
         <f aca="false">J228+D228</f>
@@ -11753,7 +11758,7 @@
         <v>2.3125</v>
       </c>
       <c r="N229" s="1" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="O229" s="3" t="n">
         <v>1</v>
@@ -11767,10 +11772,10 @@
     </row>
     <row r="230" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B230" s="44" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
       <c r="C230" s="38" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
       <c r="D230" s="38" t="n">
         <v>6</v>
@@ -11786,7 +11791,7 @@
         <v>27</v>
       </c>
       <c r="I230" s="38" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="J230" s="45" t="n">
         <f aca="false">J229+D229</f>
@@ -11805,7 +11810,7 @@
         <v>2.46875</v>
       </c>
       <c r="N230" s="1" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="O230" s="3" t="n">
         <v>1</v>
@@ -11819,10 +11824,10 @@
     </row>
     <row r="231" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B231" s="44" t="s">
-        <v>482</v>
+        <v>483</v>
       </c>
       <c r="C231" s="38" t="s">
-        <v>482</v>
+        <v>483</v>
       </c>
       <c r="D231" s="38" t="n">
         <v>6</v>
@@ -11838,7 +11843,7 @@
         <v>27</v>
       </c>
       <c r="I231" s="38" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="J231" s="45" t="n">
         <f aca="false">J230+D230</f>
@@ -11857,7 +11862,7 @@
         <v>2.65625</v>
       </c>
       <c r="N231" s="1" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="O231" s="3" t="n">
         <v>1</v>
@@ -11871,10 +11876,10 @@
     </row>
     <row r="232" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B232" s="44" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="C232" s="38" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="D232" s="38" t="n">
         <v>5</v>
@@ -11890,7 +11895,7 @@
         <v>27</v>
       </c>
       <c r="I232" s="38" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="J232" s="45" t="n">
         <f aca="false">J231+D231</f>
@@ -11909,7 +11914,7 @@
         <v>2.84375</v>
       </c>
       <c r="N232" s="1" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="O232" s="3" t="n">
         <v>1</v>
@@ -11923,7 +11928,7 @@
     </row>
     <row r="233" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A233" s="1" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
       <c r="B233" s="44"/>
       <c r="C233" s="38"/>
@@ -11940,10 +11945,10 @@
     </row>
     <row r="234" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B234" s="44" t="s">
-        <v>485</v>
+        <v>486</v>
       </c>
       <c r="C234" s="38" t="s">
-        <v>485</v>
+        <v>486</v>
       </c>
       <c r="D234" s="38" t="n">
         <v>8</v>
@@ -11959,7 +11964,7 @@
         <v>71</v>
       </c>
       <c r="I234" s="38" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="J234" s="45" t="n">
         <f aca="false">J232+D232</f>
@@ -11978,7 +11983,7 @@
         <v>3</v>
       </c>
       <c r="N234" s="1" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="O234" s="3" t="n">
         <v>1</v>
@@ -11992,10 +11997,10 @@
     </row>
     <row r="235" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B235" s="44" t="s">
-        <v>486</v>
+        <v>487</v>
       </c>
       <c r="C235" s="38" t="s">
-        <v>486</v>
+        <v>487</v>
       </c>
       <c r="D235" s="38" t="n">
         <v>8</v>
@@ -12011,7 +12016,7 @@
         <v>71</v>
       </c>
       <c r="I235" s="38" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="J235" s="45" t="n">
         <f aca="false">J234+D234</f>
@@ -12030,7 +12035,7 @@
         <v>3.25</v>
       </c>
       <c r="N235" s="1" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="O235" s="3" t="n">
         <v>1</v>
@@ -12044,10 +12049,10 @@
     </row>
     <row r="236" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B236" s="44" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
       <c r="C236" s="38" t="s">
-        <v>488</v>
+        <v>489</v>
       </c>
       <c r="D236" s="38" t="n">
         <v>16</v>
@@ -12063,7 +12068,7 @@
         <v>27</v>
       </c>
       <c r="I236" s="38" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="J236" s="45" t="n">
         <f aca="false">J235+D235</f>
@@ -12105,7 +12110,7 @@
       <c r="G237" s="38"/>
       <c r="H237" s="38"/>
       <c r="I237" s="38" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="J237" s="45" t="n">
         <f aca="false">J236+D236</f>
@@ -12126,7 +12131,7 @@
     </row>
     <row r="238" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A238" s="43" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
       <c r="F238" s="38"/>
       <c r="G238" s="38"/>
@@ -12210,10 +12215,10 @@
     </row>
     <row r="241" s="48" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B241" s="21" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="C241" s="46" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="D241" s="1" t="n">
         <v>5</v>
@@ -12229,7 +12234,7 @@
         <v>27</v>
       </c>
       <c r="I241" s="38" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="J241" s="45" t="n">
         <f aca="false">J237</f>
@@ -12262,10 +12267,10 @@
     </row>
     <row r="242" s="48" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B242" s="21" t="s">
-        <v>492</v>
+        <v>493</v>
       </c>
       <c r="C242" s="46" t="s">
-        <v>493</v>
+        <v>494</v>
       </c>
       <c r="D242" s="1" t="n">
         <v>1</v>
@@ -12275,13 +12280,13 @@
       </c>
       <c r="F242" s="47"/>
       <c r="G242" s="38" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="H242" s="38" t="s">
         <v>27</v>
       </c>
       <c r="I242" s="38" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="J242" s="45" t="n">
         <f aca="false">J241+D241</f>
@@ -12300,7 +12305,7 @@
         <v>4.15625</v>
       </c>
       <c r="N242" s="1" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="O242" s="3" t="n">
         <v>1</v>
@@ -12314,10 +12319,10 @@
     </row>
     <row r="243" s="48" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B243" s="21" t="s">
-        <v>494</v>
+        <v>495</v>
       </c>
       <c r="C243" s="46" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
       <c r="D243" s="1" t="n">
         <v>1</v>
@@ -12327,13 +12332,13 @@
       </c>
       <c r="F243" s="47"/>
       <c r="G243" s="38" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="H243" s="38" t="s">
         <v>27</v>
       </c>
       <c r="I243" s="38" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="J243" s="45" t="n">
         <f aca="false">J242+D242</f>
@@ -12352,7 +12357,7 @@
         <v>4.1875</v>
       </c>
       <c r="N243" s="1" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c r="O243" s="3" t="n">
         <v>2</v>
@@ -12366,10 +12371,10 @@
     </row>
     <row r="244" s="48" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B244" s="21" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="C244" s="46" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="D244" s="1" t="n">
         <v>3</v>
@@ -12385,7 +12390,7 @@
         <v>27</v>
       </c>
       <c r="I244" s="38" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="J244" s="45" t="n">
         <f aca="false">J243+D243</f>
@@ -12404,7 +12409,7 @@
         <v>4.21875</v>
       </c>
       <c r="N244" s="1" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c r="O244" s="3" t="n">
         <v>2</v>
@@ -12418,10 +12423,10 @@
     </row>
     <row r="245" s="48" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B245" s="21" t="s">
-        <v>499</v>
+        <v>500</v>
       </c>
       <c r="C245" s="46" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="D245" s="1" t="n">
         <v>4</v>
@@ -12431,13 +12436,13 @@
       </c>
       <c r="F245" s="47"/>
       <c r="G245" s="38" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="H245" s="38" t="s">
         <v>27</v>
       </c>
       <c r="I245" s="38" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="J245" s="45" t="n">
         <f aca="false">J244+D244</f>
@@ -12456,7 +12461,7 @@
         <v>4.3125</v>
       </c>
       <c r="N245" s="1" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c r="O245" s="3" t="n">
         <v>2</v>
@@ -12470,10 +12475,10 @@
     </row>
     <row r="246" s="48" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B246" s="21" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="C246" s="46" t="s">
-        <v>503</v>
+        <v>504</v>
       </c>
       <c r="D246" s="1" t="n">
         <v>4</v>
@@ -12483,13 +12488,13 @@
       </c>
       <c r="F246" s="47"/>
       <c r="G246" s="38" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="H246" s="38" t="s">
         <v>27</v>
       </c>
       <c r="I246" s="38" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="J246" s="45" t="n">
         <f aca="false">J245+D245</f>
@@ -12508,7 +12513,7 @@
         <v>4.4375</v>
       </c>
       <c r="N246" s="1" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c r="O246" s="3" t="n">
         <v>2</v>
@@ -12522,10 +12527,10 @@
     </row>
     <row r="247" s="48" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B247" s="21" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
       <c r="C247" s="46" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
       <c r="D247" s="1" t="n">
         <v>5</v>
@@ -12535,13 +12540,13 @@
       </c>
       <c r="F247" s="47"/>
       <c r="G247" s="38" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
       <c r="H247" s="38" t="s">
         <v>27</v>
       </c>
       <c r="I247" s="38" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="J247" s="45" t="n">
         <f aca="false">J246+D246</f>
@@ -12560,7 +12565,7 @@
         <v>4.5625</v>
       </c>
       <c r="N247" s="1" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c r="O247" s="3" t="n">
         <v>2</v>
@@ -12574,10 +12579,10 @@
     </row>
     <row r="248" s="48" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B248" s="21" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
       <c r="C248" s="46" t="s">
-        <v>508</v>
+        <v>509</v>
       </c>
       <c r="D248" s="1" t="n">
         <v>9</v>
@@ -12593,7 +12598,7 @@
         <v>27</v>
       </c>
       <c r="I248" s="38" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="J248" s="45" t="n">
         <f aca="false">J247+D247</f>
@@ -12612,7 +12617,7 @@
         <v>4.71875</v>
       </c>
       <c r="N248" s="1" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c r="O248" s="3" t="n">
         <v>2</v>
@@ -12645,10 +12650,10 @@
     </row>
     <row r="250" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B250" s="48" t="s">
-        <v>509</v>
+        <v>510</v>
       </c>
       <c r="C250" s="3" t="s">
-        <v>510</v>
+        <v>511</v>
       </c>
       <c r="D250" s="1" t="n">
         <v>8</v>
@@ -12664,7 +12669,7 @@
         <v>27</v>
       </c>
       <c r="I250" s="38" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="J250" s="45" t="n">
         <f aca="false">J248+D248</f>
@@ -12683,7 +12688,7 @@
         <v>5</v>
       </c>
       <c r="N250" s="1" t="s">
-        <v>511</v>
+        <v>512</v>
       </c>
       <c r="O250" s="3" t="n">
         <v>3</v>
@@ -12697,10 +12702,10 @@
     </row>
     <row r="251" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B251" s="48" t="s">
-        <v>512</v>
+        <v>513</v>
       </c>
       <c r="C251" s="3" t="s">
-        <v>513</v>
+        <v>514</v>
       </c>
       <c r="D251" s="1" t="n">
         <v>8</v>
@@ -12716,7 +12721,7 @@
         <v>27</v>
       </c>
       <c r="I251" s="38" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="J251" s="45" t="n">
         <f aca="false">J250+D250</f>
@@ -12735,7 +12740,7 @@
         <v>5.25</v>
       </c>
       <c r="N251" s="1" t="s">
-        <v>511</v>
+        <v>512</v>
       </c>
       <c r="O251" s="3" t="n">
         <v>3</v>
@@ -12749,10 +12754,10 @@
     </row>
     <row r="252" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B252" s="48" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
       <c r="C252" s="3" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
       <c r="D252" s="1" t="n">
         <v>8</v>
@@ -12768,7 +12773,7 @@
         <v>27</v>
       </c>
       <c r="I252" s="38" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="J252" s="45" t="n">
         <f aca="false">J251+D251</f>
@@ -12787,7 +12792,7 @@
         <v>5.5</v>
       </c>
       <c r="N252" s="1" t="s">
-        <v>511</v>
+        <v>512</v>
       </c>
       <c r="O252" s="3" t="n">
         <v>3</v>
@@ -12801,10 +12806,10 @@
     </row>
     <row r="253" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B253" s="48" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
       <c r="C253" s="3" t="s">
-        <v>517</v>
+        <v>518</v>
       </c>
       <c r="D253" s="1" t="n">
         <v>8</v>
@@ -12820,7 +12825,7 @@
         <v>27</v>
       </c>
       <c r="I253" s="38" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="J253" s="45" t="n">
         <f aca="false">J252+D252</f>
@@ -12839,7 +12844,7 @@
         <v>5.75</v>
       </c>
       <c r="N253" s="1" t="s">
-        <v>511</v>
+        <v>512</v>
       </c>
       <c r="O253" s="3" t="n">
         <v>3</v>
@@ -12853,10 +12858,10 @@
     </row>
     <row r="254" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B254" s="48" t="s">
-        <v>518</v>
+        <v>519</v>
       </c>
       <c r="C254" s="3" t="s">
-        <v>519</v>
+        <v>520</v>
       </c>
       <c r="D254" s="1" t="n">
         <v>8</v>
@@ -12872,7 +12877,7 @@
         <v>27</v>
       </c>
       <c r="I254" s="38" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="J254" s="45" t="n">
         <f aca="false">J253+D253</f>
@@ -12891,7 +12896,7 @@
         <v>6</v>
       </c>
       <c r="N254" s="1" t="s">
-        <v>511</v>
+        <v>512</v>
       </c>
       <c r="O254" s="3" t="n">
         <v>3</v>
@@ -12905,10 +12910,10 @@
     </row>
     <row r="255" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B255" s="48" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
       <c r="C255" s="3" t="s">
-        <v>521</v>
+        <v>522</v>
       </c>
       <c r="D255" s="1" t="n">
         <v>8</v>
@@ -12924,7 +12929,7 @@
         <v>27</v>
       </c>
       <c r="I255" s="38" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="J255" s="45" t="n">
         <f aca="false">J254+D254</f>
@@ -12943,7 +12948,7 @@
         <v>6.25</v>
       </c>
       <c r="N255" s="1" t="s">
-        <v>511</v>
+        <v>512</v>
       </c>
       <c r="O255" s="3" t="n">
         <v>3</v>
@@ -12957,10 +12962,10 @@
     </row>
     <row r="256" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B256" s="48" t="s">
-        <v>522</v>
+        <v>523</v>
       </c>
       <c r="C256" s="3" t="s">
-        <v>523</v>
+        <v>524</v>
       </c>
       <c r="D256" s="1" t="n">
         <v>8</v>
@@ -12976,7 +12981,7 @@
         <v>27</v>
       </c>
       <c r="I256" s="38" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="J256" s="45" t="n">
         <f aca="false">J255+D255</f>
@@ -12995,7 +13000,7 @@
         <v>6.5</v>
       </c>
       <c r="N256" s="1" t="s">
-        <v>511</v>
+        <v>512</v>
       </c>
       <c r="O256" s="3" t="n">
         <v>3</v>
@@ -13009,10 +13014,10 @@
     </row>
     <row r="257" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B257" s="48" t="s">
-        <v>524</v>
+        <v>525</v>
       </c>
       <c r="C257" s="3" t="s">
-        <v>525</v>
+        <v>526</v>
       </c>
       <c r="D257" s="1" t="n">
         <v>8</v>
@@ -13028,7 +13033,7 @@
         <v>27</v>
       </c>
       <c r="I257" s="38" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="J257" s="45" t="n">
         <f aca="false">J256+D256</f>
@@ -13047,7 +13052,7 @@
         <v>6.75</v>
       </c>
       <c r="N257" s="1" t="s">
-        <v>511</v>
+        <v>512</v>
       </c>
       <c r="O257" s="3" t="n">
         <v>3</v>
@@ -13061,10 +13066,10 @@
     </row>
     <row r="258" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B258" s="48" t="s">
-        <v>526</v>
+        <v>527</v>
       </c>
       <c r="C258" s="3" t="s">
-        <v>526</v>
+        <v>527</v>
       </c>
       <c r="D258" s="1" t="n">
         <v>8</v>
@@ -13080,7 +13085,7 @@
         <v>27</v>
       </c>
       <c r="I258" s="38" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="J258" s="45" t="n">
         <f aca="false">J257+D257</f>
@@ -13099,7 +13104,7 @@
         <v>7</v>
       </c>
       <c r="N258" s="1" t="s">
-        <v>511</v>
+        <v>512</v>
       </c>
       <c r="O258" s="3" t="n">
         <v>3</v>
@@ -13113,10 +13118,10 @@
     </row>
     <row r="259" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B259" s="48" t="s">
-        <v>527</v>
+        <v>528</v>
       </c>
       <c r="C259" s="3" t="s">
-        <v>527</v>
+        <v>528</v>
       </c>
       <c r="D259" s="1" t="n">
         <v>8</v>
@@ -13132,7 +13137,7 @@
         <v>27</v>
       </c>
       <c r="I259" s="38" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="J259" s="45" t="n">
         <f aca="false">J258+D258</f>
@@ -13151,7 +13156,7 @@
         <v>7.25</v>
       </c>
       <c r="N259" s="1" t="s">
-        <v>511</v>
+        <v>512</v>
       </c>
       <c r="O259" s="3" t="n">
         <v>3</v>
@@ -13165,10 +13170,10 @@
     </row>
     <row r="260" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B260" s="48" t="s">
-        <v>528</v>
+        <v>529</v>
       </c>
       <c r="C260" s="3" t="s">
-        <v>528</v>
+        <v>529</v>
       </c>
       <c r="D260" s="1" t="n">
         <v>8</v>
@@ -13184,7 +13189,7 @@
         <v>27</v>
       </c>
       <c r="I260" s="38" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="J260" s="45" t="n">
         <f aca="false">J259+D259</f>
@@ -13203,7 +13208,7 @@
         <v>7.5</v>
       </c>
       <c r="N260" s="1" t="s">
-        <v>511</v>
+        <v>512</v>
       </c>
       <c r="O260" s="3" t="n">
         <v>3</v>
@@ -13217,10 +13222,10 @@
     </row>
     <row r="261" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B261" s="48" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="C261" s="3" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="D261" s="1" t="n">
         <v>8</v>
@@ -13236,7 +13241,7 @@
         <v>27</v>
       </c>
       <c r="I261" s="38" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="J261" s="45" t="n">
         <f aca="false">J260+D260</f>
@@ -13255,7 +13260,7 @@
         <v>7.75</v>
       </c>
       <c r="N261" s="1" t="s">
-        <v>511</v>
+        <v>512</v>
       </c>
       <c r="O261" s="3" t="n">
         <v>3</v>
@@ -13269,10 +13274,10 @@
     </row>
     <row r="262" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B262" s="48" t="s">
-        <v>530</v>
+        <v>531</v>
       </c>
       <c r="C262" s="3" t="s">
-        <v>530</v>
+        <v>531</v>
       </c>
       <c r="D262" s="1" t="n">
         <v>8</v>
@@ -13288,7 +13293,7 @@
         <v>27</v>
       </c>
       <c r="I262" s="38" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="J262" s="45" t="n">
         <f aca="false">J261+D261</f>
@@ -13307,7 +13312,7 @@
         <v>8</v>
       </c>
       <c r="N262" s="1" t="s">
-        <v>511</v>
+        <v>512</v>
       </c>
       <c r="O262" s="3" t="n">
         <v>3</v>
@@ -13321,10 +13326,10 @@
     </row>
     <row r="263" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B263" s="48" t="s">
-        <v>531</v>
+        <v>532</v>
       </c>
       <c r="C263" s="3" t="s">
-        <v>532</v>
+        <v>533</v>
       </c>
       <c r="D263" s="1" t="n">
         <v>16</v>
@@ -13342,7 +13347,7 @@
         <v>27</v>
       </c>
       <c r="I263" s="38" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="J263" s="45" t="n">
         <f aca="false">J262+D262</f>
@@ -13361,7 +13366,7 @@
         <v>8.25</v>
       </c>
       <c r="N263" s="1" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="O263" s="3" t="n">
         <v>1</v>
@@ -13375,10 +13380,10 @@
     </row>
     <row r="264" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B264" s="48" t="s">
-        <v>533</v>
+        <v>534</v>
       </c>
       <c r="C264" s="3" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="D264" s="1" t="n">
         <v>8</v>
@@ -13394,7 +13399,7 @@
         <v>27</v>
       </c>
       <c r="I264" s="38" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="J264" s="45" t="n">
         <f aca="false">J263+D263</f>
@@ -13413,7 +13418,7 @@
         <v>8.75</v>
       </c>
       <c r="N264" s="1" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c r="O264" s="3" t="n">
         <v>2</v>
@@ -13502,7 +13507,7 @@
   <dimension ref="B6:Q1031"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C33" activeCellId="1" sqref="G56:G59 C33"/>
+      <selection pane="topLeft" activeCell="C33" activeCellId="0" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -13517,22 +13522,22 @@
     <row r="6" s="51" customFormat="true" ht="34.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B6" s="52"/>
       <c r="C6" s="52" t="s">
-        <v>535</v>
+        <v>536</v>
       </c>
       <c r="D6" s="52" t="s">
-        <v>536</v>
+        <v>537</v>
       </c>
       <c r="E6" s="52" t="s">
-        <v>537</v>
+        <v>538</v>
       </c>
       <c r="F6" s="52" t="s">
-        <v>538</v>
+        <v>539</v>
       </c>
       <c r="G6" s="52" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="H6" s="52" t="s">
-        <v>539</v>
+        <v>540</v>
       </c>
       <c r="I6" s="52"/>
     </row>
@@ -13902,10 +13907,10 @@
     </row>
     <row r="26" s="1" customFormat="true" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="32" t="s">
-        <v>540</v>
+        <v>541</v>
       </c>
       <c r="C26" s="32" t="s">
-        <v>541</v>
+        <v>542</v>
       </c>
       <c r="D26" s="27" t="n">
         <v>16</v>
@@ -13918,10 +13923,10 @@
         <v>1</v>
       </c>
       <c r="H26" s="3" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="I26" s="28" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="J26" s="29" t="n">
         <f aca="false">DownlinkSpecLTM!J169+DownlinkSpecLTM!D169</f>
@@ -13940,7 +13945,7 @@
         <v>15.5</v>
       </c>
       <c r="N26" s="1" t="s">
-        <v>542</v>
+        <v>543</v>
       </c>
       <c r="O26" s="3" t="n">
         <v>6</v>
@@ -13954,10 +13959,10 @@
     </row>
     <row r="27" s="1" customFormat="true" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="32" t="s">
-        <v>543</v>
+        <v>544</v>
       </c>
       <c r="C27" s="32" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="D27" s="27" t="n">
         <v>32</v>
@@ -13968,10 +13973,10 @@
         <v>1</v>
       </c>
       <c r="H27" s="3" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="I27" s="28" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="J27" s="29" t="n">
         <f aca="false">J26+D26</f>
@@ -13990,7 +13995,7 @@
         <v>16</v>
       </c>
       <c r="N27" s="1" t="s">
-        <v>542</v>
+        <v>543</v>
       </c>
       <c r="O27" s="3" t="n">
         <v>6</v>
@@ -14004,16 +14009,16 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="50" t="s">
-        <v>545</v>
+        <v>546</v>
       </c>
       <c r="C30" s="50" t="s">
-        <v>546</v>
+        <v>547</v>
       </c>
       <c r="D30" s="50" t="s">
-        <v>547</v>
+        <v>548</v>
       </c>
       <c r="E30" s="50" t="s">
-        <v>548</v>
+        <v>549</v>
       </c>
       <c r="F30" s="50"/>
     </row>

</xml_diff>

<commit_message>
Final (I hope) update for MESAT1
Add RSSI and forward power conversions
</commit_message>
<xml_diff>
--- a/genSpacecraft/DownlinkSpecMESAT1.xlsx
+++ b/genSpacecraft/DownlinkSpecMESAT1.xlsx
@@ -479,7 +479,7 @@
     <t xml:space="preserve">FwdPower</t>
   </si>
   <si>
-    <t xml:space="preserve">icr_8bit_volts|txv2_fwd_pwr|dBm_to_mW</t>
+    <t xml:space="preserve">mesat_power_out</t>
   </si>
   <si>
     <t xml:space="preserve">Receiver card temperature</t>
@@ -491,7 +491,7 @@
     <t xml:space="preserve">rssi</t>
   </si>
   <si>
-    <t xml:space="preserve">icr_8bit_volts|icrv2_rssi </t>
+    <t xml:space="preserve">mesat_rssi</t>
   </si>
   <si>
     <t xml:space="preserve">dBm</t>
@@ -2048,8 +2048,8 @@
   </sheetPr>
   <dimension ref="A1:Q1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A56" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H69" activeCellId="0" sqref="H69"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A39" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G50" activeCellId="0" sqref="G50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4066,7 +4066,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="25.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B50" s="31" t="s">
         <v>150</v>
       </c>

</xml_diff>

<commit_message>
Did not include the source file for previous changes
</commit_message>
<xml_diff>
--- a/genSpacecraft/DownlinkSpecMESAT1.xlsx
+++ b/genSpacecraft/DownlinkSpecMESAT1.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1462" uniqueCount="550">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1464" uniqueCount="550">
   <si>
     <t xml:space="preserve">//</t>
   </si>
@@ -851,7 +851,7 @@
     <t xml:space="preserve">wodSize</t>
   </si>
   <si>
-    <t xml:space="preserve">Number of WOD data payloads kept for each of Science and Housekeeping.  In hundreds</t>
+    <t xml:space="preserve">Number of WOD data payloads kept for each type (Housekeeping in MESat1)</t>
   </si>
   <si>
     <t xml:space="preserve">Diagnostic</t>
@@ -2048,8 +2048,8 @@
   </sheetPr>
   <dimension ref="A1:Q1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A39" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G50" activeCellId="0" sqref="G50"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A88" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L236" activeCellId="0" sqref="L236"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6455,7 +6455,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" customFormat="false" ht="75.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="100" customFormat="false" ht="64.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B100" s="31" t="s">
         <v>274</v>
       </c>
@@ -9703,8 +9703,8 @@
         <v>402</v>
       </c>
       <c r="F170" s="23"/>
-      <c r="G170" s="23" t="n">
-        <v>36</v>
+      <c r="G170" s="23" t="s">
+        <v>161</v>
       </c>
       <c r="H170" s="22" t="s">
         <v>27</v>
@@ -9839,7 +9839,7 @@
       <c r="E176" s="38"/>
       <c r="F176" s="23"/>
       <c r="G176" s="39" t="n">
-        <v>36</v>
+        <v>0</v>
       </c>
       <c r="H176" s="0"/>
       <c r="I176" s="28" t="s">
@@ -9983,7 +9983,7 @@
       <c r="E179" s="38"/>
       <c r="F179" s="23"/>
       <c r="G179" s="39" t="n">
-        <v>36</v>
+        <v>0</v>
       </c>
       <c r="I179" s="28" t="s">
         <v>430</v>
@@ -10031,8 +10031,8 @@
         <v>402</v>
       </c>
       <c r="F180" s="23"/>
-      <c r="G180" s="23" t="n">
-        <v>36</v>
+      <c r="G180" s="23" t="s">
+        <v>161</v>
       </c>
       <c r="H180" s="22" t="s">
         <v>27</v>

</xml_diff>

<commit_message>
Change to use "invalid_check" function.
</commit_message>
<xml_diff>
--- a/genSpacecraft/DownlinkSpecMESAT1.xlsx
+++ b/genSpacecraft/DownlinkSpecMESAT1.xlsx
@@ -374,7 +374,7 @@
     <t xml:space="preserve">uint8_t</t>
   </si>
   <si>
-    <t xml:space="preserve">MESAT1_BATT_TEMP_TABLE|INVALID_10K</t>
+    <t xml:space="preserve">mesat_batt_temp|invalid_check(280 Invalid 0)</t>
   </si>
   <si>
     <t xml:space="preserve">Host Temp 1</t>
@@ -542,7 +542,7 @@
     <t xml:space="preserve">MinusYTemp</t>
   </si>
   <si>
-    <t xml:space="preserve">8_bit_temp|INVALID_TEMP</t>
+    <t xml:space="preserve">8_bit_temp|invalid_check(107.5 Invalid 1)</t>
   </si>
   <si>
     <t xml:space="preserve">Minus X Temp</t>
@@ -614,7 +614,7 @@
     <t xml:space="preserve">hostCANVolts0</t>
   </si>
   <si>
-    <t xml:space="preserve">TEN_VOLT_8_BIT|INVALID_10K</t>
+    <t xml:space="preserve">10_volt_8_bit|invalid_check(10 Invalid 1)</t>
   </si>
   <si>
     <t xml:space="preserve">Host Bat Volts 1</t>
@@ -647,7 +647,7 @@
     <t xml:space="preserve">hostCANVolts3</t>
   </si>
   <si>
-    <t xml:space="preserve">BATT_CURRENT|INVALID_10K</t>
+    <t xml:space="preserve">mesat_batt_current|invalid_check(2000 Invalid 0)</t>
   </si>
   <si>
     <t xml:space="preserve">Host Bat Volts 4</t>
@@ -2051,8 +2051,8 @@
   </sheetPr>
   <dimension ref="A1:Q1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E55" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G69" activeCellId="0" sqref="G69"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A78" activeCellId="0" sqref="A78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4915,7 +4915,7 @@
         <v>116</v>
       </c>
       <c r="F66" s="23"/>
-      <c r="G66" s="22" t="s">
+      <c r="G66" s="23" t="s">
         <v>197</v>
       </c>
       <c r="H66" s="22" t="s">
@@ -13510,7 +13510,7 @@
   <dimension ref="B6:Q1031"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C33" activeCellId="1" sqref="G69 C33"/>
+      <selection pane="topLeft" activeCell="C33" activeCellId="0" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Update to fix MESAT1 science telemetry
</commit_message>
<xml_diff>
--- a/genSpacecraft/DownlinkSpecMESAT1.xlsx
+++ b/genSpacecraft/DownlinkSpecMESAT1.xlsx
@@ -2051,8 +2051,8 @@
   </sheetPr>
   <dimension ref="A1:Q1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A78" activeCellId="0" sqref="A78"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A190" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D199" activeCellId="0" sqref="D199"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -10658,7 +10658,7 @@
         <v>450</v>
       </c>
       <c r="D199" s="22" t="n">
-        <v>5248</v>
+        <v>5216</v>
       </c>
       <c r="E199" s="22" t="s">
         <v>26</v>
@@ -10728,19 +10728,19 @@
       </c>
       <c r="J200" s="4" t="n">
         <f aca="false">J199+D199</f>
-        <v>5248</v>
+        <v>5216</v>
       </c>
       <c r="K200" s="28" t="n">
         <f aca="false">J200/8</f>
-        <v>656</v>
+        <v>652</v>
       </c>
       <c r="L200" s="28" t="n">
         <f aca="false">J200/16</f>
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="M200" s="28" t="n">
         <f aca="false">J200/32</f>
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="N200" s="1" t="s">
         <v>28</v>
@@ -10778,19 +10778,19 @@
       </c>
       <c r="J201" s="4" t="n">
         <f aca="false">J200+D200</f>
-        <v>5255</v>
+        <v>5223</v>
       </c>
       <c r="K201" s="28" t="n">
         <f aca="false">J201/8</f>
-        <v>656.875</v>
+        <v>652.875</v>
       </c>
       <c r="L201" s="28" t="n">
         <f aca="false">J201/16</f>
-        <v>328.4375</v>
+        <v>326.4375</v>
       </c>
       <c r="M201" s="28" t="n">
         <f aca="false">J201/32</f>
-        <v>164.21875</v>
+        <v>163.21875</v>
       </c>
       <c r="N201" s="1" t="s">
         <v>457</v>
@@ -10814,19 +10814,19 @@
       </c>
       <c r="J202" s="4" t="n">
         <f aca="false">J201+D201</f>
-        <v>5256</v>
+        <v>5224</v>
       </c>
       <c r="K202" s="28" t="n">
         <f aca="false">J202/8</f>
-        <v>657</v>
+        <v>653</v>
       </c>
       <c r="L202" s="28" t="n">
         <f aca="false">J202/16</f>
-        <v>328.5</v>
+        <v>326.5</v>
       </c>
       <c r="M202" s="28" t="n">
         <f aca="false">J202/32</f>
-        <v>164.25</v>
+        <v>163.25</v>
       </c>
     </row>
     <row r="203" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Update the MESAT telemetry defs
New definitions from UMaine.  Also bug in long science which overwrote CRC
and overflow bit.

Use a new conversion curves file for LTM since UMaine was not following the
spec and we needed a different curve.
</commit_message>
<xml_diff>
--- a/genSpacecraft/DownlinkSpecMESAT1.xlsx
+++ b/genSpacecraft/DownlinkSpecMESAT1.xlsx
@@ -614,7 +614,7 @@
     <t xml:space="preserve">hostCANVolts0</t>
   </si>
   <si>
-    <t xml:space="preserve">10_volt_8_bit|invalid_check(10 Invalid 1)</t>
+    <t xml:space="preserve">8dot4_volt_8_bit</t>
   </si>
   <si>
     <t xml:space="preserve">Host Bat Volts 1</t>
@@ -626,7 +626,7 @@
     <t xml:space="preserve">hostCANVolts1</t>
   </si>
   <si>
-    <t xml:space="preserve">mesat_batt_capacity</t>
+    <t xml:space="preserve">MESAT1BatSOC|batsoc</t>
   </si>
   <si>
     <t xml:space="preserve">Host Bat Volts 2</t>
@@ -680,7 +680,7 @@
     <t xml:space="preserve">Host Voltage 7</t>
   </si>
   <si>
-    <t xml:space="preserve">Unused  6</t>
+    <t xml:space="preserve">BckBtmLft Temp</t>
   </si>
   <si>
     <t xml:space="preserve">hostI2cTemp0</t>
@@ -689,34 +689,34 @@
     <t xml:space="preserve">Interior Temp</t>
   </si>
   <si>
-    <t xml:space="preserve">BckBtmLft Temp</t>
+    <t xml:space="preserve">Other MESAT1 Telemetry</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Front Ctr Temp</t>
   </si>
   <si>
     <t xml:space="preserve">hostI2cTemp1</t>
   </si>
   <si>
-    <t xml:space="preserve">Other MESAT1 Telemetry</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Front Ctr Temp</t>
+    <t xml:space="preserve">BckTopLft Temp</t>
   </si>
   <si>
     <t xml:space="preserve">hostI2cTemp2</t>
   </si>
   <si>
-    <t xml:space="preserve">BckTopLft Temp</t>
+    <t xml:space="preserve">FrontBtmLft Temp</t>
   </si>
   <si>
     <t xml:space="preserve">hostI2cTemp3</t>
   </si>
   <si>
-    <t xml:space="preserve">FrontBtmLft Temp</t>
+    <t xml:space="preserve">BckTopRgt Temp</t>
   </si>
   <si>
     <t xml:space="preserve">hostI2cTemp4</t>
   </si>
   <si>
-    <t xml:space="preserve">BckTopRgt Temp</t>
+    <t xml:space="preserve">Unused 6</t>
   </si>
   <si>
     <t xml:space="preserve">hostI2cTemp5</t>
@@ -2051,8 +2051,8 @@
   </sheetPr>
   <dimension ref="A1:Q1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A190" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D199" activeCellId="0" sqref="D199"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A56" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G66" activeCellId="0" sqref="G66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2068,7 +2068,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="18.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="4" width="8.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="11" style="5" width="8.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="18.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="39.55"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="3" width="8.97"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="13.22"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="17" style="1" width="8.73"/>
@@ -3907,7 +3907,7 @@
         <v>7</v>
       </c>
       <c r="P46" s="1" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="Q46" s="1" t="n">
         <v>3</v>
@@ -4421,16 +4421,16 @@
         <v>7</v>
       </c>
       <c r="N56" s="1" t="s">
-        <v>136</v>
+        <v>28</v>
       </c>
       <c r="O56" s="3" t="n">
         <v>7</v>
       </c>
       <c r="P56" s="1" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="Q56" s="1" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="25.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4577,16 +4577,16 @@
         <v>7.75</v>
       </c>
       <c r="N59" s="1" t="s">
-        <v>136</v>
+        <v>28</v>
       </c>
       <c r="O59" s="3" t="n">
         <v>7</v>
       </c>
       <c r="P59" s="1" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="Q59" s="1" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="37.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4687,7 +4687,7 @@
         <v>7</v>
       </c>
       <c r="P61" s="1" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="Q61" s="1" t="n">
         <v>3</v>
@@ -4739,7 +4739,7 @@
         <v>7</v>
       </c>
       <c r="P62" s="1" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="Q62" s="1" t="n">
         <v>4</v>
@@ -4895,7 +4895,7 @@
         <v>7</v>
       </c>
       <c r="P65" s="1" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="Q65" s="1" t="n">
         <v>3</v>
@@ -5298,24 +5298,24 @@
         <v>11.25</v>
       </c>
       <c r="N73" s="1" t="s">
-        <v>28</v>
+        <v>222</v>
       </c>
       <c r="O73" s="24" t="n">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="P73" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q73" s="1" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B74" s="31" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="C74" s="32" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="D74" s="32" t="n">
         <v>8</v>
@@ -5350,13 +5350,13 @@
         <v>11.5</v>
       </c>
       <c r="N74" s="1" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="O74" s="24" t="n">
         <v>9</v>
       </c>
       <c r="P74" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Q74" s="1" t="n">
         <v>3</v>
@@ -5402,13 +5402,13 @@
         <v>11.75</v>
       </c>
       <c r="N75" s="1" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="O75" s="24" t="n">
         <v>9</v>
       </c>
       <c r="P75" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="Q75" s="1" t="n">
         <v>3</v>
@@ -5454,13 +5454,13 @@
         <v>12</v>
       </c>
       <c r="N76" s="1" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="O76" s="24" t="n">
         <v>9</v>
       </c>
       <c r="P76" s="1" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="Q76" s="1" t="n">
         <v>3</v>
@@ -5506,13 +5506,13 @@
         <v>12.25</v>
       </c>
       <c r="N77" s="1" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="O77" s="24" t="n">
         <v>9</v>
       </c>
       <c r="P77" s="1" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="Q77" s="1" t="n">
         <v>3</v>
@@ -5558,16 +5558,16 @@
         <v>12.5</v>
       </c>
       <c r="N78" s="1" t="s">
-        <v>224</v>
+        <v>42</v>
       </c>
       <c r="O78" s="24" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="P78" s="1" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="Q78" s="1" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5662,7 +5662,7 @@
         <v>13</v>
       </c>
       <c r="N80" s="1" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="O80" s="24" t="n">
         <v>9</v>
@@ -6708,7 +6708,7 @@
         <v>16.75</v>
       </c>
       <c r="N104" s="1" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="O104" s="3" t="n">
         <v>9</v>
@@ -7864,7 +7864,7 @@
         <v>17.6875</v>
       </c>
       <c r="N127" s="1" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="O127" s="24" t="n">
         <v>9</v>
@@ -7914,7 +7914,7 @@
         <v>17.71875</v>
       </c>
       <c r="N128" s="1" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="O128" s="24" t="n">
         <v>9</v>
@@ -8270,7 +8270,7 @@
         <v>7</v>
       </c>
       <c r="P135" s="1" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="Q135" s="1" t="n">
         <v>0</v>

</xml_diff>